<commit_message>
Add Excel RACI matrix template for stakeholder responsibilities
</commit_message>
<xml_diff>
--- a/01_Stakeholder_Alignment/templates/RACI_Matrix_Template.xlsx
+++ b/01_Stakeholder_Alignment/templates/RACI_Matrix_Template.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivana\Desktop\AI_Operating_Model_Transformation\01_Stakeholder_Alignment\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E99EFE-CA89-4DAC-ACAC-2546C4C85831}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="27">
   <si>
     <t>Activity</t>
   </si>
@@ -80,13 +86,75 @@
   </si>
   <si>
     <t>R/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Legend </t>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Accountable (final decision-maker)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Consulted (input provider)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Informed (needs to be kept in the loop)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = Responsible (does the work)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,16 +170,43 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -134,14 +229,258 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -149,13 +488,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -193,7 +540,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -227,6 +574,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -261,9 +609,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -436,273 +785,330 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="15.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
+      <c r="D2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="E3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
+      <c r="G3" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E4" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
+      <c r="G4" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="B5" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
+      <c r="F5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="B6" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="H6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" t="s">
+      <c r="H6" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B7" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="E7" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="G7" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" t="s">
+      <c r="G7" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="B8" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" t="s">
+    <row r="9" spans="1:9" s="1" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="B9" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="H9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" t="s">
-        <v>18</v>
-      </c>
+      <c r="H9" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="9"/>
+      <c r="D12" s="10"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="7"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="7"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="13"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="7"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>